<commit_message>
Included localfile for OpenZeppelin dependencies.
</commit_message>
<xml_diff>
--- a/tools/Gas estimation.xlsx
+++ b/tools/Gas estimation.xlsx
@@ -477,7 +477,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +531,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="2">
-        <f>IF(D4&lt;&gt;"",D4*0.000000001,"")</f>
+        <f t="shared" ref="F4:F17" si="0">IF(D4&lt;&gt;"",D4*0.000000001,"")</f>
         <v>0.31034970500000003</v>
       </c>
     </row>
@@ -546,7 +546,7 @@
         <v>95</v>
       </c>
       <c r="D5" s="9">
-        <f t="shared" ref="D5:D17" si="0">IF(AND(B5&lt;&gt;"",C5&lt;&gt;""),B5*C5,"")</f>
+        <f t="shared" ref="D5:D17" si="1">IF(AND(B5&lt;&gt;"",C5&lt;&gt;""),B5*C5,"")</f>
         <v>287647840</v>
       </c>
       <c r="E5" s="9">
@@ -554,7 +554,7 @@
         <v>-22701865</v>
       </c>
       <c r="F5" s="2">
-        <f>IF(D5&lt;&gt;"",D5*0.000000001,"")</f>
+        <f t="shared" si="0"/>
         <v>0.28764784000000004</v>
       </c>
     </row>
@@ -569,15 +569,15 @@
         <v>81</v>
       </c>
       <c r="D6" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>220391766</v>
       </c>
       <c r="E6" s="9" t="str">
-        <f t="shared" ref="E6:E17" si="1">IF(D6&lt;&gt;"",IF(C6=C5,D6-D5,"--"),"")</f>
+        <f t="shared" ref="E6:E17" si="2">IF(D6&lt;&gt;"",IF(C6=C5,D6-D5,"--"),"")</f>
         <v>--</v>
       </c>
       <c r="F6" s="2">
-        <f>IF(D6&lt;&gt;"",D6*0.000000001,"")</f>
+        <f t="shared" si="0"/>
         <v>0.22039176600000002</v>
       </c>
     </row>
@@ -590,15 +590,15 @@
         <v>81</v>
       </c>
       <c r="D7" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>220391766</v>
       </c>
       <c r="E7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F7" s="2">
-        <f>IF(D7&lt;&gt;"",D7*0.000000001,"")</f>
+        <f t="shared" si="0"/>
         <v>0.22039176600000002</v>
       </c>
     </row>
@@ -611,15 +611,15 @@
         <v>81</v>
       </c>
       <c r="D8" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>245257632</v>
       </c>
       <c r="E8" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24865866</v>
       </c>
       <c r="F8" s="2">
-        <f>IF(D8&lt;&gt;"",D8*0.000000001,"")</f>
+        <f t="shared" si="0"/>
         <v>0.245257632</v>
       </c>
     </row>
@@ -632,15 +632,15 @@
         <v>81</v>
       </c>
       <c r="D9" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>247128327</v>
       </c>
       <c r="E9" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1870695</v>
       </c>
       <c r="F9" s="2">
-        <f>IF(D9&lt;&gt;"",D9*0.000000001,"")</f>
+        <f t="shared" si="0"/>
         <v>0.24712832700000001</v>
       </c>
     </row>
@@ -653,15 +653,15 @@
         <v>81</v>
       </c>
       <c r="D10" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>251809479</v>
       </c>
       <c r="E10" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4681152</v>
       </c>
       <c r="F10" s="2">
-        <f>IF(D10&lt;&gt;"",D10*0.000000001,"")</f>
+        <f t="shared" si="0"/>
         <v>0.251809479</v>
       </c>
     </row>
@@ -674,15 +674,15 @@
         <v>68</v>
       </c>
       <c r="D11" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>209256060</v>
       </c>
       <c r="E11" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>--</v>
       </c>
       <c r="F11" s="2">
-        <f>IF(D11&lt;&gt;"",D11*0.000000001,"")</f>
+        <f t="shared" si="0"/>
         <v>0.20925606000000002</v>
       </c>
     </row>
@@ -695,33 +695,37 @@
         <v>70</v>
       </c>
       <c r="D12" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>215410650</v>
       </c>
       <c r="E12" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>--</v>
       </c>
       <c r="F12" s="2">
-        <f>IF(D12&lt;&gt;"",D12*0.000000001,"")</f>
+        <f t="shared" si="0"/>
         <v>0.21541065000000001</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E13" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F13" s="2" t="str">
-        <f>IF(D13&lt;&gt;"",D13*0.000000001,"")</f>
-        <v/>
+      <c r="B13" s="6">
+        <v>3077271</v>
+      </c>
+      <c r="C13" s="1">
+        <v>70</v>
+      </c>
+      <c r="D13" s="9">
+        <f t="shared" si="1"/>
+        <v>215408970</v>
+      </c>
+      <c r="E13" s="9">
+        <f t="shared" si="2"/>
+        <v>-1680</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.21540897000000001</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -729,15 +733,15 @@
       <c r="B14" s="6"/>
       <c r="C14" s="1"/>
       <c r="D14" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E14" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F14" s="2" t="str">
-        <f>IF(D14&lt;&gt;"",D14*0.000000001,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -746,15 +750,15 @@
       <c r="B15" s="6"/>
       <c r="C15" s="1"/>
       <c r="D15" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E15" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F15" s="2" t="str">
-        <f>IF(D15&lt;&gt;"",D15*0.000000001,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -763,15 +767,15 @@
       <c r="B16" s="6"/>
       <c r="C16" s="1"/>
       <c r="D16" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E16" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F16" s="2" t="str">
-        <f>IF(D16&lt;&gt;"",D16*0.000000001,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -780,15 +784,15 @@
       <c r="B17" s="6"/>
       <c r="C17" s="1"/>
       <c r="D17" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E17" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F17" s="2" t="str">
-        <f>IF(D17&lt;&gt;"",D17*0.000000001,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
- Replaced require statements by revert errors clauses - At burn(), fixed the amount comparison with balance, since amount is in token units, and balanceOf uses decimals.
</commit_message>
<xml_diff>
--- a/tools/Gas estimation.xlsx
+++ b/tools/Gas estimation.xlsx
@@ -474,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,52 +751,378 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="9" t="str">
+      <c r="B15" s="6">
+        <v>3077295</v>
+      </c>
+      <c r="C15" s="1">
+        <v>41</v>
+      </c>
+      <c r="D15" s="9">
         <f t="shared" si="1"/>
-        <v/>
+        <v>126169095</v>
       </c>
       <c r="E15" s="9" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="F15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <v>--</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.12616909500000001</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="9" t="str">
+      <c r="B16" s="6">
+        <v>2944022</v>
+      </c>
+      <c r="C16" s="1">
+        <v>38</v>
+      </c>
+      <c r="D16" s="9">
         <f t="shared" si="1"/>
-        <v/>
+        <v>111872836</v>
       </c>
       <c r="E16" s="9" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="F16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <v>--</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="0"/>
+        <v>0.111872836</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="9" t="str">
+      <c r="B17" s="6">
+        <v>2944022</v>
+      </c>
+      <c r="C17" s="1">
+        <v>38</v>
+      </c>
+      <c r="D17" s="9">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E17" s="9" t="str">
+        <v>111872836</v>
+      </c>
+      <c r="E17" s="9">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="F17" s="2" t="str">
-        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.111872836</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="6">
+        <v>2691648</v>
+      </c>
+      <c r="C18" s="1">
+        <v>38</v>
+      </c>
+      <c r="D18" s="9">
+        <f t="shared" ref="D18:D35" si="3">IF(AND(B18&lt;&gt;"",C18&lt;&gt;""),B18*C18,"")</f>
+        <v>102282624</v>
+      </c>
+      <c r="E18" s="9">
+        <f t="shared" ref="E18:E35" si="4">IF(D18&lt;&gt;"",IF(C18=C17,D18-D17,"--"),"")</f>
+        <v>-9590212</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" ref="F18:F35" si="5">IF(D18&lt;&gt;"",D18*0.000000001,"")</f>
+        <v>0.102282624</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="6">
+        <v>2607152</v>
+      </c>
+      <c r="C19" s="1">
+        <v>38</v>
+      </c>
+      <c r="D19" s="9">
+        <f t="shared" si="3"/>
+        <v>99071776</v>
+      </c>
+      <c r="E19" s="9">
+        <f t="shared" si="4"/>
+        <v>-3210848</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" si="5"/>
+        <v>9.9071776E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E20" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F20" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E21" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F21" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E22" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F22" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F23" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E24" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F24" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E25" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F25" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E26" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F26" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E27" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F27" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E28" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F28" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E29" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F29" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E30" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F30" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E31" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F31" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E32" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F32" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E33" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F33" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E34" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F34" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E35" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F35" s="2" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Merged runInflation with tuneInflation because there was a semaphore which could lead to concurrent critical path, which could lead to reentrancy possibility.
</commit_message>
<xml_diff>
--- a/tools/Gas estimation.xlsx
+++ b/tools/Gas estimation.xlsx
@@ -477,7 +477,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,7 +855,9 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="A20" s="4">
+        <v>45062.953591550926</v>
+      </c>
       <c r="B20" s="6"/>
       <c r="C20" s="1"/>
       <c r="D20" s="9" t="str">

</xml_diff>